<commit_message>
[IMP] Adjust Input Tax Report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_input_tax.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_input_tax.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Input Tax Report" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t xml:space="preserve">Input Tax Report</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t xml:space="preserve">Taxbranch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run By</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run Date</t>
   </si>
   <si>
     <t xml:space="preserve">Item</t>
@@ -68,8 +74,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="#,###.00"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -177,7 +185,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -186,12 +194,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -206,10 +214,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -226,10 +230,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -240,14 +240,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -335,45 +327,44 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:7"/>
+  <dimension ref="A1:AMJ9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.3979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="17.3979591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="17.3979591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="3" width="17.3979591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="2" width="17.3979591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.3979591836735"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="4" width="17.3979591836735"/>
-    <col collapsed="false" hidden="false" max="1023" min="14" style="5" width="17.3979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="17.3979591836735"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="1" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="3" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="10" style="4" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="14" style="5" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="17.4"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="7" customFormat="true" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -383,115 +374,149 @@
       <c r="M2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="17" t="s">
+      <c r="A6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="B8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="E8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="F8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="AMJ6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17"/>
-      <c r="B7" s="19" t="s">
+      <c r="G8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="H8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="19" t="s">
+      <c r="I8" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="AMJ8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="C9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="17"/>
-      <c r="AMJ7" s="5"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="14"/>
+      <c r="AMJ9" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:I9"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.3" right="0.3" top="0.609722222222222" bottom="0.370138888888889" header="0.511805555555555" footer="0.1"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter>&amp;L&amp;8 2018-02-20 09:37:39&amp;R&amp;8&amp;P / &amp;N</oddFooter>

</xml_diff>